<commit_message>
"Some Changes in Workflow"
</commit_message>
<xml_diff>
--- a/all data.xlsx
+++ b/all data.xlsx
@@ -33,6 +33,9 @@
     <t>Location</t>
   </si>
   <si>
+    <t>ImageLink</t>
+  </si>
+  <si>
     <t>Website</t>
   </si>
   <si>
@@ -42,6 +45,9 @@
     <t>Hours</t>
   </si>
   <si>
+    <t>Images</t>
+  </si>
+  <si>
     <t xml:space="preserve"> BUSINESS SARTHI  </t>
   </si>
   <si>
@@ -54,7 +60,7 @@
     <t xml:space="preserve">       A-67, Block C, Sector 2, Noida, Uttar Pradesh 201301      </t>
   </si>
   <si>
-    <t>https://i.postimg.cc/gcHHLQ0m/1map.png</t>
+    <t>https://i.postimg.cc/9fwWRQDD/1map.png</t>
   </si>
   <si>
     <t xml:space="preserve">       businesssarthi.org      </t>
@@ -96,7 +102,7 @@
     <t xml:space="preserve">       B 96, B Block, Sector 65, Noida, Uttar Pradesh 201301      </t>
   </si>
   <si>
-    <t>https://i.postimg.cc/RZgZjYHT/3map.png</t>
+    <t>https://i.postimg.cc/sfZDqtMy/3map.png</t>
   </si>
   <si>
     <t xml:space="preserve">       witsourcetechnology.com      </t>
@@ -105,7 +111,7 @@
     <t>088009 60940</t>
   </si>
   <si>
-    <t xml:space="preserve">       Open ⋅ Closes 6PM        </t>
+    <t xml:space="preserve">       Closes soon ⋅ 6PM ⋅ Opens 10AM Wed        </t>
   </si>
   <si>
     <t xml:space="preserve"> business consultant  </t>
@@ -156,13 +162,13 @@
     <t xml:space="preserve">       B-42, 3rd Floor, B Block, Sector 65, Noida, Uttar Pradesh 201301      </t>
   </si>
   <si>
-    <t>https://i.postimg.cc/k5Mf52Dm/6map.png</t>
+    <t>https://i.postimg.cc/V6W4k76N/6map.png</t>
   </si>
   <si>
     <t xml:space="preserve">       pristinebs.com      </t>
   </si>
   <si>
-    <t xml:space="preserve">       Open ⋅ Closes 6:30PM        </t>
+    <t xml:space="preserve">       Closes soon ⋅ 6:30PM ⋅ Opens 10AM Wed        </t>
   </si>
   <si>
     <t xml:space="preserve"> Jha Group Of Services  </t>
@@ -192,7 +198,7 @@
     <t xml:space="preserve">       A - 38 K, Block A, Sector 64, Noida, Uttar Pradesh 201301      </t>
   </si>
   <si>
-    <t>https://i.postimg.cc/sgLvM8gg/8map.png</t>
+    <t>https://i.postimg.cc/505xxKry/8map.png</t>
   </si>
   <si>
     <t xml:space="preserve">       myoffice-hub.com      </t>
@@ -220,12 +226,6 @@
   </si>
   <si>
     <t xml:space="preserve">       Open ⋅ Closes 7:30PM        </t>
-  </si>
-  <si>
-    <t>Image Link</t>
-  </si>
-  <si>
-    <t>Images</t>
   </si>
 </sst>
 </file>
@@ -321,16 +321,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -360,76 +360,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>514350</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -716,12 +646,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,258 +681,258 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>19</v>
+        <v>54</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1019,34 +949,5 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
-  <drawing r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
-  <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" dvAspect="DVASPECT_ICON" shapeId="1025" r:id="rId13">
-          <objectPr defaultSize="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>514350</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Packager Shell Object" dvAspect="DVASPECT_ICON" shapeId="1025" r:id="rId13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </oleObjects>
 </worksheet>
 </file>
</xml_diff>